<commit_message>
Added ability to populate item group if specified
</commit_message>
<xml_diff>
--- a/products_example.xlsx
+++ b/products_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\github\citrus-lime-cloudmt-product-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0DECE3-793C-49F7-A7C4-2646C6796650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89F6143-927F-4F23-9230-55897347A163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31679887-9772-44D4-9908-4C3D13F38678}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{31679887-9772-44D4-9908-4C3D13F38678}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Item Lookup Code</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>DETECT</t>
+  </si>
+  <si>
+    <t>Item Group</t>
+  </si>
+  <si>
+    <t>Feed</t>
   </si>
 </sst>
 </file>
@@ -133,9 +139,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -173,7 +179,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -279,7 +285,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -421,7 +427,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3BC738-4EE5-4114-ABD7-1264833B6F71}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,9 +449,10 @@
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +471,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -483,6 +493,9 @@
       </c>
       <c r="F2" t="b">
         <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -495,5 +508,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>